<commit_message>
fix empty row in spreadsheet
</commit_message>
<xml_diff>
--- a/other_files/Cycorp claims.xlsx
+++ b/other_files/Cycorp claims.xlsx
@@ -478,10 +478,10 @@
         <color rgb="FF284E3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF284E3F"/>
@@ -489,13 +489,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF284E3F"/>
@@ -503,13 +503,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
         <color rgb="FF284E3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF284E3F"/>
@@ -519,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -565,13 +565,37 @@
     <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -583,37 +607,10 @@
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -711,12 +708,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$43</c:f>
+              <c:f>Sheet1!$A$2:$A$42</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$43</c:f>
+              <c:f>Sheet1!$D$2:$D$42</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -740,12 +737,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$43</c:f>
+              <c:f>Sheet1!$A$2:$A$42</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$43</c:f>
+              <c:f>Sheet1!$E$2:$E$42</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -769,12 +766,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$43</c:f>
+              <c:f>Sheet1!$A$2:$A$42</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$43</c:f>
+              <c:f>Sheet1!$F$2:$F$42</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -804,22 +801,22 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$43</c:f>
+              <c:f>Sheet1!$A$2:$A$42</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$43</c:f>
+              <c:f>Sheet1!$K$2:$K$42</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="224899564"/>
-        <c:axId val="1550715936"/>
+        <c:axId val="1315409790"/>
+        <c:axId val="2142471079"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="224899564"/>
+        <c:axId val="1315409790"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -871,10 +868,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1550715936"/>
+        <c:crossAx val="2142471079"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1550715936"/>
+        <c:axId val="2142471079"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -949,7 +946,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224899564"/>
+        <c:crossAx val="1315409790"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -981,7 +978,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1600200</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
@@ -1006,7 +1003,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:N43" displayName="Table1" name="Table1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:N42" displayName="Table1" name="Table1" id="1">
   <tableColumns count="14">
     <tableColumn name="time" id="1"/>
     <tableColumn name="predicates (in K)" id="2"/>
@@ -1535,12 +1532,12 @@
     </row>
     <row r="11">
       <c r="A11" s="10">
-        <v>33543.0</v>
+        <v>34090.0</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="14">
-        <v>1.5</v>
+        <v>1.0</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -1549,56 +1546,60 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="15"/>
+      <c r="L11" s="12">
+        <v>30.0</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5">
-        <v>34090.0</v>
+        <v>34425.0</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="7">
-        <v>1.0</v>
-      </c>
+      <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
+      <c r="G12" s="7">
+        <v>40.0</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="8">
-        <v>30.0</v>
-      </c>
       <c r="M12" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="10">
-        <v>34425.0</v>
+        <v>34700.0</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
+      <c r="D13" s="14">
+        <v>0.4</v>
+      </c>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="14">
-        <v>40.0</v>
-      </c>
+      <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="M13" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14">
@@ -1606,91 +1607,93 @@
         <v>34700.0</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+      <c r="C14" s="7">
+        <v>100.0</v>
+      </c>
       <c r="D14" s="7">
-        <v>0.4</v>
+        <v>1.0</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="J14" s="7">
+        <v>2005.0</v>
+      </c>
+      <c r="K14" s="7">
+        <v>10.0</v>
+      </c>
       <c r="M14" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="10">
+      <c r="A15" s="15">
         <v>34700.0</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="14">
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="G15" s="16"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="16">
+        <v>10.0</v>
+      </c>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N15" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5">
+        <v>34943.0</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7">
         <v>100.0</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D16" s="7">
         <v>1.0</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="14">
-        <v>2005.0</v>
-      </c>
-      <c r="K15" s="14">
-        <v>10.0</v>
-      </c>
-      <c r="M15" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="N15" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="16">
-        <v>34700.0</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17">
-        <v>1.0</v>
-      </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="17">
-        <v>10.0</v>
-      </c>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="N16" s="21" t="s">
-        <v>37</v>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="M16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="10">
-        <v>34943.0</v>
+        <v>35604.0</v>
       </c>
       <c r="B17" s="11"/>
-      <c r="C17" s="14">
-        <v>100.0</v>
-      </c>
+      <c r="C17" s="11"/>
       <c r="D17" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E17" s="11"/>
+        <v>2.0</v>
+      </c>
+      <c r="E17" s="14">
+        <v>4.0</v>
+      </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
@@ -1698,70 +1701,72 @@
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
       <c r="M17" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="N17" s="13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="5">
-        <v>35604.0</v>
+        <v>35796.0</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="E18" s="7">
-        <v>4.0</v>
-      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
+      <c r="L18" s="8">
+        <v>40.0</v>
+      </c>
       <c r="M18" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="10">
-        <v>35796.0</v>
+        <v>36957.0</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+      <c r="E19" s="14">
+        <v>4.5</v>
+      </c>
+      <c r="F19" s="14">
+        <v>5.0</v>
+      </c>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
-      <c r="L19" s="12">
-        <v>40.0</v>
-      </c>
       <c r="M19" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N19" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="5">
-        <v>36957.0</v>
+        <v>37063.0</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="D20" s="21">
+        <v>1.4</v>
+      </c>
       <c r="E20" s="7">
-        <v>4.5</v>
+        <v>5.0</v>
       </c>
       <c r="F20" s="7">
         <v>5.0</v>
@@ -1772,641 +1777,614 @@
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="M20" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="10">
-        <v>37063.0</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="22">
+      <c r="A21" s="15">
+        <v>37135.0</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="16">
+        <v>2011.0</v>
+      </c>
+      <c r="K21" s="16">
+        <v>10.0</v>
+      </c>
+      <c r="L21" s="22"/>
+      <c r="M21" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="N21" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="23">
+        <v>37347.0</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="26">
+        <v>1.5</v>
+      </c>
+      <c r="E22" s="25">
+        <v>6.0</v>
+      </c>
+      <c r="F22" s="25">
+        <v>6.0</v>
+      </c>
+      <c r="G22" s="25"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="N22" s="29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="15">
+        <v>37354.0</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="16">
+        <v>300.0</v>
+      </c>
+      <c r="D23" s="17">
+        <v>3.0</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16">
+        <v>6.0</v>
+      </c>
+      <c r="G23" s="16">
+        <v>100.0</v>
+      </c>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="16">
+        <v>2007.0</v>
+      </c>
+      <c r="K23" s="16">
+        <v>5.0</v>
+      </c>
+      <c r="L23" s="22"/>
+      <c r="M23" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="N23" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="23">
+        <v>37414.0</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="26">
         <v>1.4</v>
       </c>
-      <c r="E21" s="14">
-        <v>5.0</v>
-      </c>
-      <c r="F21" s="14">
-        <v>5.0</v>
-      </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="M21" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="N21" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="16">
-        <v>37135.0</v>
-      </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="18">
-        <v>1.5</v>
-      </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="17">
-        <v>2011.0</v>
-      </c>
-      <c r="K22" s="17">
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="N24" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="15">
+        <v>37987.0</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="16">
+        <v>155.0</v>
+      </c>
+      <c r="D25" s="17">
+        <v>2.5</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="N25" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="23">
+        <v>38353.0</v>
+      </c>
+      <c r="B26" s="25">
+        <v>15.0</v>
+      </c>
+      <c r="C26" s="25">
+        <v>250.0</v>
+      </c>
+      <c r="D26" s="26">
+        <v>2.2</v>
+      </c>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="N26" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="15">
+        <v>38353.0</v>
+      </c>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="16">
+        <v>2015.0</v>
+      </c>
+      <c r="K27" s="16">
         <v>10.0</v>
       </c>
-      <c r="L22" s="23"/>
-      <c r="M22" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="N22" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="24">
-        <v>37347.0</v>
-      </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="27">
-        <v>1.5</v>
-      </c>
-      <c r="E23" s="26">
-        <v>6.0</v>
-      </c>
-      <c r="F23" s="26">
-        <v>6.0</v>
-      </c>
-      <c r="G23" s="26"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="N23" s="30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="16">
-        <v>37354.0</v>
-      </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="17">
+      <c r="L27" s="22"/>
+      <c r="M27" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="N27" s="20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="23">
+        <v>38718.0</v>
+      </c>
+      <c r="B28" s="25">
+        <v>15.0</v>
+      </c>
+      <c r="C28" s="25">
+        <v>250.0</v>
+      </c>
+      <c r="D28" s="26">
+        <v>2.2</v>
+      </c>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="N28" s="29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="15">
+        <v>38718.0</v>
+      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16">
+        <v>9.0</v>
+      </c>
+      <c r="G29" s="16"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="N29" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="23">
+        <v>38822.0</v>
+      </c>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25">
         <v>300.0</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D30" s="26">
         <v>3.0</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17">
-        <v>6.0</v>
-      </c>
-      <c r="G24" s="17">
-        <v>100.0</v>
-      </c>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="17">
-        <v>2007.0</v>
-      </c>
-      <c r="K24" s="17">
-        <v>5.0</v>
-      </c>
-      <c r="L24" s="23"/>
-      <c r="M24" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="N24" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="24">
-        <v>37414.0</v>
-      </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="27">
-        <v>1.4</v>
-      </c>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="N25" s="30" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="16">
-        <v>37987.0</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="17">
-        <v>155.0</v>
-      </c>
-      <c r="D26" s="18">
-        <v>2.5</v>
-      </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="N26" s="21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="24">
-        <v>38353.0</v>
-      </c>
-      <c r="B27" s="26">
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="N30" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="15">
+        <v>38867.0</v>
+      </c>
+      <c r="B31" s="16">
         <v>15.0</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C31" s="16">
+        <v>300.0</v>
+      </c>
+      <c r="D31" s="17">
+        <v>3.2</v>
+      </c>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N31" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="23">
+        <v>39083.0</v>
+      </c>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="26">
+        <v>4.6</v>
+      </c>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="N32" s="29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="15">
+        <v>39093.0</v>
+      </c>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="19">
+        <v>1102.0</v>
+      </c>
+      <c r="M33" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="N33" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="23">
+        <v>39539.0</v>
+      </c>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="28">
+        <v>1000.0</v>
+      </c>
+      <c r="M34" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N34" s="29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="15">
+        <v>39814.0</v>
+      </c>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16">
+        <v>7.5</v>
+      </c>
+      <c r="G35" s="16"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="19">
+        <v>720.0</v>
+      </c>
+      <c r="M35" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="N35" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="23">
+        <v>40179.0</v>
+      </c>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25">
         <v>250.0</v>
       </c>
-      <c r="D27" s="27">
-        <v>2.2</v>
-      </c>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="N27" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="16">
-        <v>38353.0</v>
-      </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="17">
-        <v>2015.0</v>
-      </c>
-      <c r="K28" s="17">
+      <c r="D36" s="26">
+        <v>4.5</v>
+      </c>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25">
+        <v>9.0</v>
+      </c>
+      <c r="G36" s="25"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="N36" s="29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="15">
+        <v>41897.0</v>
+      </c>
+      <c r="B37" s="16">
+        <v>32.0</v>
+      </c>
+      <c r="C37" s="16">
+        <v>700.0</v>
+      </c>
+      <c r="D37" s="17">
+        <v>13.0</v>
+      </c>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="N37" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="23">
+        <v>42346.0</v>
+      </c>
+      <c r="B38" s="25">
+        <v>32.0</v>
+      </c>
+      <c r="C38" s="25">
+        <v>700.0</v>
+      </c>
+      <c r="D38" s="26">
+        <v>15.0</v>
+      </c>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25">
+        <v>16.0</v>
+      </c>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="25">
+        <v>2016.0</v>
+      </c>
+      <c r="K38" s="25">
+        <v>1.0</v>
+      </c>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="N38" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="15">
+        <v>42443.0</v>
+      </c>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="16">
+        <v>2016.0</v>
+      </c>
+      <c r="K39" s="16">
+        <v>0.0</v>
+      </c>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="N39" s="20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="23">
+        <v>42736.0</v>
+      </c>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="26">
+        <v>21.0</v>
+      </c>
+      <c r="E40" s="25">
+        <v>12.0</v>
+      </c>
+      <c r="F40" s="25">
         <v>10.0</v>
       </c>
-      <c r="L28" s="23"/>
-      <c r="M28" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="N28" s="21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="24">
-        <v>38718.0</v>
-      </c>
-      <c r="B29" s="26">
-        <v>15.0</v>
-      </c>
-      <c r="C29" s="26">
-        <v>250.0</v>
-      </c>
-      <c r="D29" s="27">
-        <v>2.2</v>
-      </c>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="N29" s="30" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="16">
-        <v>38718.0</v>
-      </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17">
-        <v>9.0</v>
-      </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="N30" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="24">
-        <v>38822.0</v>
-      </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26">
-        <v>300.0</v>
-      </c>
-      <c r="D31" s="27">
-        <v>3.0</v>
-      </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="N31" s="30" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="16">
-        <v>38867.0</v>
-      </c>
-      <c r="B32" s="17">
-        <v>15.0</v>
-      </c>
-      <c r="C32" s="17">
-        <v>300.0</v>
-      </c>
-      <c r="D32" s="18">
-        <v>3.2</v>
-      </c>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="N32" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="24">
-        <v>39083.0</v>
-      </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="27">
-        <v>4.6</v>
-      </c>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="N33" s="30" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="16">
-        <v>39093.0</v>
-      </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="20">
-        <v>1102.0</v>
-      </c>
-      <c r="M34" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="N34" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="24">
-        <v>39539.0</v>
-      </c>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="29">
-        <v>1000.0</v>
-      </c>
-      <c r="M35" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="N35" s="30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="16">
-        <v>39814.0</v>
-      </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17">
-        <v>7.5</v>
-      </c>
-      <c r="G36" s="17"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="20">
-        <v>720.0</v>
-      </c>
-      <c r="M36" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="N36" s="21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="24">
-        <v>40179.0</v>
-      </c>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26">
-        <v>250.0</v>
-      </c>
-      <c r="D37" s="27">
-        <v>4.5</v>
-      </c>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26">
-        <v>9.0</v>
-      </c>
-      <c r="G37" s="26"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="26"/>
-      <c r="K37" s="26"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="N37" s="30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="16">
-        <v>41897.0</v>
-      </c>
-      <c r="B38" s="17">
-        <v>32.0</v>
-      </c>
-      <c r="C38" s="17">
-        <v>700.0</v>
-      </c>
-      <c r="D38" s="18">
-        <v>13.0</v>
-      </c>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="N38" s="21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="24">
-        <v>42346.0</v>
-      </c>
-      <c r="B39" s="26">
-        <v>32.0</v>
-      </c>
-      <c r="C39" s="26">
-        <v>700.0</v>
-      </c>
-      <c r="D39" s="27">
-        <v>15.0</v>
-      </c>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26">
-        <v>16.0</v>
-      </c>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="26">
-        <v>2016.0</v>
-      </c>
-      <c r="K39" s="26">
-        <v>1.0</v>
-      </c>
-      <c r="L39" s="29"/>
-      <c r="M39" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="N39" s="30" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="16">
-        <v>42443.0</v>
-      </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="17">
-        <v>2016.0</v>
-      </c>
-      <c r="K40" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="N40" s="21" t="s">
-        <v>85</v>
+      <c r="G40" s="25"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="N40" s="29" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="24">
-        <v>42736.0</v>
-      </c>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="27">
-        <v>21.0</v>
-      </c>
-      <c r="E41" s="26">
-        <v>12.0</v>
-      </c>
-      <c r="F41" s="26">
-        <v>10.0</v>
-      </c>
-      <c r="G41" s="26"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="26"/>
-      <c r="K41" s="26"/>
-      <c r="L41" s="29"/>
-      <c r="M41" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="N41" s="30" t="s">
-        <v>87</v>
+      <c r="A41" s="15">
+        <v>43466.0</v>
+      </c>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="16">
+        <v>20.0</v>
+      </c>
+      <c r="F41" s="16">
+        <v>20.0</v>
+      </c>
+      <c r="G41" s="16"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="N41" s="20" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="16">
-        <v>43466.0</v>
-      </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="17">
+      <c r="A42" s="31">
+        <v>44562.0</v>
+      </c>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="33">
+        <v>30.0</v>
+      </c>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32">
         <v>20.0</v>
       </c>
-      <c r="F42" s="17">
-        <v>20.0</v>
-      </c>
-      <c r="G42" s="17"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="17"/>
-      <c r="K42" s="17"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="N42" s="21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="32">
-        <v>44562.0</v>
-      </c>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="34">
-        <v>30.0</v>
-      </c>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33">
-        <v>20.0</v>
-      </c>
-      <c r="G43" s="33"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="33"/>
-      <c r="K43" s="33"/>
-      <c r="L43" s="36">
+      <c r="G42" s="32"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="32"/>
+      <c r="L42" s="35">
         <v>1100.0</v>
       </c>
-      <c r="M43" s="36" t="s">
+      <c r="M42" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="N43" s="37" t="s">
+      <c r="N42" s="36" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A43">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A42">
       <formula1>OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:K43">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:K42">
       <formula1>AND(ISNUMBER(B2),(NOT(OR(NOT(ISERROR(DATEVALUE(B2))), AND(ISNUMBER(B2), LEFT(CELL("format", B2))="D")))))</formula1>
     </dataValidation>
   </dataValidations>
@@ -2420,38 +2398,38 @@
     <hyperlink r:id="rId7" ref="N8"/>
     <hyperlink r:id="rId8" ref="N9"/>
     <hyperlink r:id="rId9" ref="N10"/>
-    <hyperlink r:id="rId10" ref="N12"/>
-    <hyperlink r:id="rId11" ref="N13"/>
-    <hyperlink r:id="rId12" ref="N14"/>
-    <hyperlink r:id="rId13" ref="N15"/>
-    <hyperlink r:id="rId14" ref="N16"/>
-    <hyperlink r:id="rId15" ref="N17"/>
-    <hyperlink r:id="rId16" ref="N18"/>
-    <hyperlink r:id="rId17" ref="N19"/>
-    <hyperlink r:id="rId18" ref="N20"/>
-    <hyperlink r:id="rId19" ref="N21"/>
-    <hyperlink r:id="rId20" ref="N22"/>
-    <hyperlink r:id="rId21" ref="N23"/>
-    <hyperlink r:id="rId22" ref="N24"/>
-    <hyperlink r:id="rId23" ref="N25"/>
-    <hyperlink r:id="rId24" ref="N26"/>
-    <hyperlink r:id="rId25" ref="N27"/>
-    <hyperlink r:id="rId26" ref="N28"/>
-    <hyperlink r:id="rId27" ref="N29"/>
-    <hyperlink r:id="rId28" ref="N30"/>
-    <hyperlink r:id="rId29" ref="N31"/>
-    <hyperlink r:id="rId30" ref="N32"/>
-    <hyperlink r:id="rId31" ref="N33"/>
-    <hyperlink r:id="rId32" ref="N34"/>
-    <hyperlink r:id="rId33" ref="N35"/>
-    <hyperlink r:id="rId34" ref="N36"/>
-    <hyperlink r:id="rId35" ref="N37"/>
-    <hyperlink r:id="rId36" ref="N38"/>
-    <hyperlink r:id="rId37" ref="N39"/>
-    <hyperlink r:id="rId38" ref="N40"/>
-    <hyperlink r:id="rId39" ref="N41"/>
-    <hyperlink r:id="rId40" ref="N42"/>
-    <hyperlink r:id="rId41" ref="N43"/>
+    <hyperlink r:id="rId10" ref="N11"/>
+    <hyperlink r:id="rId11" ref="N12"/>
+    <hyperlink r:id="rId12" ref="N13"/>
+    <hyperlink r:id="rId13" ref="N14"/>
+    <hyperlink r:id="rId14" ref="N15"/>
+    <hyperlink r:id="rId15" ref="N16"/>
+    <hyperlink r:id="rId16" ref="N17"/>
+    <hyperlink r:id="rId17" ref="N18"/>
+    <hyperlink r:id="rId18" ref="N19"/>
+    <hyperlink r:id="rId19" ref="N20"/>
+    <hyperlink r:id="rId20" ref="N21"/>
+    <hyperlink r:id="rId21" ref="N22"/>
+    <hyperlink r:id="rId22" ref="N23"/>
+    <hyperlink r:id="rId23" ref="N24"/>
+    <hyperlink r:id="rId24" ref="N25"/>
+    <hyperlink r:id="rId25" ref="N26"/>
+    <hyperlink r:id="rId26" ref="N27"/>
+    <hyperlink r:id="rId27" ref="N28"/>
+    <hyperlink r:id="rId28" ref="N29"/>
+    <hyperlink r:id="rId29" ref="N30"/>
+    <hyperlink r:id="rId30" ref="N31"/>
+    <hyperlink r:id="rId31" ref="N32"/>
+    <hyperlink r:id="rId32" ref="N33"/>
+    <hyperlink r:id="rId33" ref="N34"/>
+    <hyperlink r:id="rId34" ref="N35"/>
+    <hyperlink r:id="rId35" ref="N36"/>
+    <hyperlink r:id="rId36" ref="N37"/>
+    <hyperlink r:id="rId37" ref="N38"/>
+    <hyperlink r:id="rId38" ref="N39"/>
+    <hyperlink r:id="rId39" ref="N40"/>
+    <hyperlink r:id="rId40" ref="N41"/>
+    <hyperlink r:id="rId41" ref="N42"/>
   </hyperlinks>
   <drawing r:id="rId42"/>
   <tableParts count="1">

</xml_diff>